<commit_message>
add validation tests for ODE solver; fix bug which used populations instead of concentration to validate continuous submodels; add time_step_factor to run ODEs more frequently than checkpoint time step; update a couple of validation cases; add ODE test case 00004; improve layout of plots
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/validation/cases/semantic/00014/00014-wc_lang.xlsx
+++ b/tests/multialgorithm/fixtures/validation/cases/semantic/00014/00014-wc_lang.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="420" yWindow="460" windowWidth="23700" windowHeight="7560" tabRatio="989" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="1120" yWindow="460" windowWidth="23700" windowHeight="7560" tabRatio="989" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="93">
   <si>
     <t>Id</t>
   </si>
@@ -290,9 +290,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>Basic single forward reaction with two species in one compartment</t>
-  </si>
-  <si>
     <t>S2</t>
   </si>
   <si>
@@ -338,13 +335,13 @@
     <t>k1 * S1[c] * S1[c] * S2[c]</t>
   </si>
   <si>
-    <t>k1 * S3[c]</t>
-  </si>
-  <si>
     <t>k2</t>
   </si>
   <si>
     <t>These MWs mass-balance the reactions</t>
+  </si>
+  <si>
+    <t>k2 * S3[c]</t>
   </si>
 </sst>
 </file>
@@ -831,16 +828,14 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>75</v>
-      </c>
+      <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -903,7 +898,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -942,24 +937,24 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1113,7 +1108,7 @@
         <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>71</v>
@@ -1127,10 +1122,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>71</v>
@@ -1144,10 +1139,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>71</v>
@@ -1386,7 +1381,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1474,10 +1469,10 @@
         <v>72</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>21</v>
@@ -1540,7 +1535,7 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
@@ -1616,7 +1611,7 @@
         <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2"/>
       <c r="F2" s="2">
@@ -1629,18 +1624,18 @@
         <v>29</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3"/>
       <c r="F3" s="2">
@@ -1653,18 +1648,18 @@
         <v>29</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4"/>
       <c r="F4" s="2">
@@ -1677,7 +1672,7 @@
         <v>29</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1724,7 +1719,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="14">
         <v>1E-4</v>
@@ -1737,7 +1732,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="14">
         <v>2.0000000000000001E-4</v>
@@ -1748,7 +1743,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="14">
         <v>1E-4</v>
@@ -1898,16 +1893,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>79</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" s="10">
         <v>0</v>
@@ -1919,16 +1914,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>87</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="10">
         <v>0</v>

</xml_diff>